<commit_message>
Edits to land use files based on consultation with American Forest Foundation and American Forests
</commit_message>
<xml_diff>
--- a/InputData/land/CApULAbIFM/CO2 Abated per Unit Land Area by Impr For Mgmt.xlsx
+++ b/InputData/land/CApULAbIFM/CO2 Abated per Unit Land Area by Impr For Mgmt.xlsx
@@ -1,22 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\land\CApULAbIFM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF08A53-F280-4704-83EC-0E3DACD573C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="315" windowWidth="18825" windowHeight="6555"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Calculations" sheetId="4" r:id="rId2"/>
-    <sheet name="CApULAbIFM" sheetId="3" r:id="rId3"/>
+    <sheet name="CApULAbIFM" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>CApULAbIFM CO2 Abated per Unit Land Area by Improved Forest Management</t>
   </si>
@@ -30,44 +46,14 @@
     <t>Per Acre</t>
   </si>
   <si>
-    <t>Increased Annual CO2 Sequestration Achievable by Improved Management Practices per Acre</t>
-  </si>
-  <si>
-    <t>tons CO2 / acre / yr</t>
-  </si>
-  <si>
-    <t>Low Estimate</t>
-  </si>
-  <si>
-    <t>High Estimate</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>g CO2 / acre / yr</t>
-  </si>
-  <si>
-    <t>Average, converted to grams CO2</t>
-  </si>
-  <si>
-    <t>U.S. EPA</t>
-  </si>
-  <si>
-    <t>Greenhouse Gas Mitigation Potential in U.S. Forestry and Agriculture</t>
-  </si>
-  <si>
-    <t>http://www.epa.gov/climate/climatechange/Downloads/ccs/ghg_mitigation_forestry_ag_2005.pdf</t>
-  </si>
-  <si>
-    <t>Page 2-3, Table 2-1</t>
+    <t>consultation with American Forest Foundation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,14 +65,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,24 +87,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -134,6 +107,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -182,7 +158,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -215,9 +191,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,6 +243,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -425,10 +435,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -442,120 +454,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="4">
-        <v>2005</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
+      <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:2" ht="14.45" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2.1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3.1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>AVERAGE(A2:A3)</f>
-        <v>2.6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <f>A4*10^6</f>
-        <v>2600000</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -572,8 +492,8 @@
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <f>Calculations!A6</f>
-        <v>2600000</v>
+        <f>1.5*10^6</f>
+        <v>1500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>